<commit_message>
add 'alive/dead' status to form
</commit_message>
<xml_diff>
--- a/plant_form.xlsx
+++ b/plant_form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
   <si>
     <t>type</t>
   </si>
@@ -28,6 +28,9 @@
     <t>label</t>
   </si>
   <si>
+    <t>label:es</t>
+  </si>
+  <si>
     <t>relevant</t>
   </si>
   <si>
@@ -55,6 +58,9 @@
     <t>Plant ID</t>
   </si>
   <si>
+    <t>código</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
@@ -70,12 +76,18 @@
     <t>Species</t>
   </si>
   <si>
+    <t>especie</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
     <t>Location</t>
   </si>
   <si>
+    <t>ubicación</t>
+  </si>
+  <si>
     <t>begin repeat</t>
   </si>
   <si>
@@ -85,6 +97,9 @@
     <t>add a new picture</t>
   </si>
   <si>
+    <t>otra foto</t>
+  </si>
+  <si>
     <t>image</t>
   </si>
   <si>
@@ -94,16 +109,43 @@
     <t>Picture</t>
   </si>
   <si>
+    <t>foto</t>
+  </si>
+  <si>
     <t>end repeat</t>
   </si>
   <si>
+    <t>select_one status</t>
+  </si>
+  <si>
+    <t>alive</t>
+  </si>
+  <si>
+    <t>Alive</t>
+  </si>
+  <si>
+    <t>viva</t>
+  </si>
+  <si>
     <t>note</t>
   </si>
   <si>
     <t>Note</t>
   </si>
   <si>
+    <t>notas</t>
+  </si>
+  <si>
     <t>list name</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>dead</t>
+  </si>
+  <si>
+    <t>muerta</t>
   </si>
   <si>
     <t>form_title</t>
@@ -137,8 +179,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -218,7 +261,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,6 +271,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -252,12 +303,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -278,129 +329,175 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
+      <c r="E7" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>27</v>
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -419,12 +516,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -434,13 +531,44 @@
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -461,7 +589,7 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -471,38 +599,38 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>34</v>
+      <c r="A1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="3" t="n">
+      <c r="A2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="5" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
version 4; 1/0 vs true/false
</commit_message>
<xml_diff>
--- a/plant_form.xlsx
+++ b/plant_form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="198" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -179,9 +179,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -278,7 +277,7 @@
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -518,7 +517,7 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -547,7 +546,8 @@
       <c r="A2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4" t="b">
+      <c r="B2" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -561,7 +561,8 @@
       <c r="A3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="4" t="b">
+      <c r="B3" s="4" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -589,8 +590,8 @@
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -631,7 +632,7 @@
         <v>51</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
have to change form id or it won't upload
</commit_message>
<xml_diff>
--- a/plant_form.xlsx
+++ b/plant_form.xlsx
@@ -169,7 +169,7 @@
     <t>Plant Form</t>
   </si>
   <si>
-    <t>plant_form_r</t>
+    <t>plant_form_s</t>
   </si>
   <si>
     <t>English</t>
@@ -260,7 +260,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -275,10 +275,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -546,7 +542,7 @@
       <c r="A2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -561,7 +557,7 @@
       <c r="A3" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -591,7 +587,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -600,38 +596,38 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="4" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>